<commit_message>
added new code in scheduletype code system
</commit_message>
<xml_diff>
--- a/ExampleIG/output/CodeSystem-hn-schedule-type-cs.xlsx
+++ b/ExampleIG/output/CodeSystem-hn-schedule-type-cs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-06T23:06:55+01:00</t>
+    <t>2024-11-07T10:16:17+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -111,7 +111,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>5</t>
+    <t>6</t>
   </si>
   <si>
     <t>Level</t>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Personlig</t>
+  </si>
+  <si>
+    <t>Annen"</t>
+  </si>
+  <si>
+    <t>Annen</t>
   </si>
 </sst>
 </file>
@@ -444,7 +450,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -524,6 +530,18 @@
       </c>
       <c r="D6" s="2"/>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Oppdatert kode Personel til Behandlertimebok
</commit_message>
<xml_diff>
--- a/ExampleIG/output/CodeSystem-hn-schedule-type-cs.xlsx
+++ b/ExampleIG/output/CodeSystem-hn-schedule-type-cs.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-07T10:24:13+01:00</t>
+    <t>2024-11-07T10:34:59+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -141,7 +141,7 @@
     <t>Koronatest</t>
   </si>
   <si>
-    <t>Personlig</t>
+    <t>Behandlertimebok</t>
   </si>
   <si>
     <t>Annen</t>

</xml_diff>